<commit_message>
logo afgemaakt en logboek
</commit_message>
<xml_diff>
--- a/Documentatie/logboek.xlsx
+++ b/Documentatie/logboek.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9784D6D-C6AC-427A-8EB7-C68833EA10B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA173748-56C1-4121-A852-88E23A6DC554}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Dagen</t>
   </si>
@@ -383,7 +383,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,6 +486,15 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>43606</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">

</xml_diff>